<commit_message>
Se agregaron los metodos para obtener las normas en Matriz, VectorFila y VectorColumna.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas_sel.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas_sel.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="6150" yWindow="3720" windowWidth="16380" windowHeight="8190" tabRatio="329"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="9780" tabRatio="329"/>
   </bookViews>
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -101,16 +102,22 @@
   </si>
   <si>
     <t>Operaciones algebráicas en matriz</t>
+  </si>
+  <si>
+    <t>Metodos Norma 1, 2, inf en matriz</t>
+  </si>
+  <si>
+    <t>Metodos Norma 1, 2, inf en vector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -860,17 +867,8 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -889,9 +887,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -901,7 +897,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -946,7 +941,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -1045,16 +1039,10 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-AR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1077,23 +1065,17 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-1.0204081632653062E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>1.0010204081632652</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1101,15 +1083,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.51180555555555551" footer="0.51180555555555551"/>
+    <c:pageMargins b="1" l="0.75000000000000011" r="0.75000000000000011" t="1" header="0.51180555555555562" footer="0.51180555555555562"/>
     <c:pageSetup firstPageNumber="0"/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1180,7 +1160,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1188,7 +1168,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1198,7 +1178,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1247,7 +1227,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
@@ -1255,7 +1235,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1265,7 +1245,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1588,11 +1568,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1602,7 +1582,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1630,11 +1610,11 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
@@ -1644,7 +1624,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1663,15 +1643,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:IU42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="38.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1686,7 +1666,7 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +1685,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1703,7 @@
         <v>0.84930555555555554</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1735,8 +1715,8 @@
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.5" thickBot="1"/>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>6</v>
       </c>
@@ -1768,7 +1748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15">
       <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
@@ -1802,7 +1782,7 @@
         <v>7.6388888888888618E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15">
       <c r="A7" s="18" t="s">
         <v>28</v>
       </c>
@@ -1836,43 +1816,73 @@
         <v>2.6388888888889017E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+    <row r="8" spans="1:11" ht="15">
+      <c r="A8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7">
+        <v>20</v>
+      </c>
+      <c r="C8" s="7">
+        <v>24</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.72569444444444453</v>
+      </c>
       <c r="G8" s="8">
         <f t="shared" ref="G8:G15" si="1">F8-E8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="8"/>
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <v>6.9444444444444447E-4</v>
+      </c>
       <c r="J8" s="30">
         <f t="shared" si="0"/>
+        <v>1.3888888888888952E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15">
+      <c r="A9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="7">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.7284722222222223</v>
+      </c>
+      <c r="F9" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
       <c r="G9" s="8">
         <f t="shared" si="1"/>
+        <v>-0.7284722222222223</v>
+      </c>
+      <c r="H9" s="7">
         <v>0</v>
       </c>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
       <c r="J9" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+        <v>-0.7284722222222223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15">
       <c r="A10" s="18"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1890,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15">
       <c r="A11" s="18"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1908,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15">
       <c r="A12" s="18"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1926,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15">
       <c r="A13" s="18"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1944,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15">
       <c r="A14" s="19"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1962,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
       <c r="A15" s="21"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -1980,145 +1990,145 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1">
       <c r="A16" s="48" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="24">
         <f>SUM(B6:B15)</f>
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="C16" s="24">
         <f>SUM(C6:C15)</f>
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D16" s="25">
         <f>SUM(D6:D15)</f>
-        <v>2.2222222222222223E-2</v>
+        <v>4.6527777777777779E-2</v>
       </c>
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="25">
         <f>SUM(G6:G15)</f>
-        <v>3.4027777777777879E-2</v>
+        <v>-0.68124999999999991</v>
       </c>
       <c r="H16" s="26">
         <f>SUM(H6:H15)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="27">
         <f>SUM(I6:I15)</f>
-        <v>0</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="J16" s="28">
         <f>SUM(J6:J15)</f>
-        <v>3.4027777777777879E-2</v>
+        <v>-0.68055555555555547</v>
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="15.75" thickBot="1">
       <c r="A17" s="49" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="20">
         <f>IF(EXACT($C$16, 0),"-",ABS($B$16-$C$16)/$C$16)</f>
-        <v>0.57894736842105265</v>
+        <v>0.60493827160493829</v>
       </c>
       <c r="D17" s="5"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="13.5" thickBot="1"/>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1">
       <c r="A19" s="42" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="43"/>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15">
       <c r="A20" s="31" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="32">
         <f>C16</f>
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C20" s="9"/>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15">
       <c r="A21" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="34">
         <f>IF(EXACT($B$20,0),"-",$B$20/((J16-INT(J16))*24))</f>
-        <v>69.795918367346729</v>
+        <v>10.565217391304344</v>
       </c>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1">
       <c r="A22" s="35" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="34">
         <f>IF(EXACT($B$20,0),"-",H16/($B$20/10))</f>
-        <v>0</v>
+        <v>0.1234567901234568</v>
       </c>
       <c r="C22" s="9"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1">
       <c r="A23" s="35" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="36">
         <f>IF(EXACT($B$20,0),"-",H16/$B$20)</f>
-        <v>0</v>
+        <v>1.2345679012345678E-2</v>
       </c>
       <c r="C23" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15">
       <c r="A24" s="35" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="37">
         <f>I16</f>
-        <v>0</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="C24" s="40">
         <f>IF(EXACT(J16,0),5%,B24/J16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>-1.0204081632653062E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1">
       <c r="A25" s="38" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="39">
         <f>G16</f>
-        <v>3.4027777777777879E-2</v>
+        <v>-0.68124999999999991</v>
       </c>
       <c r="C25" s="41">
         <f>IF(EXACT(J16,0),95%,B25/J16)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>1.0010204081632652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1">
       <c r="A26" s="38" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="39">
         <f>C2+C3+J16</f>
-        <v>5.0000000000000044E-2</v>
+        <v>-0.6645833333333333</v>
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="D27" s="6"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:4">
       <c r="C40" s="4"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:4">
       <c r="D42" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización de metricas_sel.xlsx con los tiempos que demore hoy.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas_sel.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas_sel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2520" windowWidth="17850" windowHeight="9780" tabRatio="329"/>
@@ -9,13 +9,12 @@
   <sheets>
     <sheet name="Metricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -108,16 +107,34 @@
   </si>
   <si>
     <t>Metodos Norma 1, 2, inf en vector</t>
+  </si>
+  <si>
+    <t>Operaciones algebráicas en VectorColumna</t>
+  </si>
+  <si>
+    <t>Operaciones algebráicas en VectorFila</t>
+  </si>
+  <si>
+    <t>Creación de la Clase MatrizCuadrada</t>
+  </si>
+  <si>
+    <t>Creación de la Clase MatrizIdentidad</t>
+  </si>
+  <si>
+    <t>Producto entre MatrizMath con VectorFila y VectorColumna</t>
+  </si>
+  <si>
+    <t>Metodos setFila y setColumna de la Clase MatrizMath</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss;@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -867,8 +884,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:date1904 val="0"/>
+  <c:lang val="es-AR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -887,7 +913,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:pieChart>
@@ -897,6 +925,7 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -941,6 +970,7 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -1039,14 +1069,20 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Metricas!$A$24:$A$25</c:f>
+              <c:f>Metricas!$A$26:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1060,22 +1096,28 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metricas!$C$24:$C$25</c:f>
+              <c:f>Metricas!$C$26:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-1.0204081632653062E-3</c:v>
+                  <c:v>-1.8018018018018014E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0010204081632652</c:v>
+                  <c:v>1.0180180180180181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
@@ -1083,9 +1125,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
@@ -1102,13 +1146,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1168,7 +1212,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1178,7 +1222,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1235,7 +1279,7 @@
         <a:effectLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="1">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="1">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="77"/>
               </a:solidFill>
@@ -1245,7 +1289,7 @@
             </a14:hiddenLine>
           </a:ext>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1582,7 +1626,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1624,7 +1668,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1643,22 +1687,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:IU42"/>
+  <dimension ref="A1:IU44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1666,7 +1710,7 @@
     <col min="11" max="255" width="34.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1729,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:11" ht="15">
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -1703,7 +1747,7 @@
         <v>0.84930555555555554</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>0</v>
       </c>
@@ -1715,8 +1759,8 @@
       <c r="D3" s="14"/>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="13.5" thickBot="1"/>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
+    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="45" t="s">
         <v>6</v>
       </c>
@@ -1748,7 +1792,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15">
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
@@ -1782,7 +1826,7 @@
         <v>7.6388888888888618E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15">
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>28</v>
       </c>
@@ -1812,11 +1856,11 @@
         <v>0</v>
       </c>
       <c r="J7" s="30">
-        <f t="shared" ref="J7:J15" si="0">G7+I7</f>
+        <f t="shared" ref="J7:J17" si="0">G7+I7</f>
         <v>2.6388888888889017E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15">
+    <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
@@ -1836,7 +1880,7 @@
         <v>0.72569444444444453</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" ref="G8:G15" si="1">F8-E8</f>
+        <f t="shared" ref="G8:G17" si="1">F8-E8</f>
         <v>1.3194444444444509E-2</v>
       </c>
       <c r="H8" s="7">
@@ -1850,7 +1894,7 @@
         <v>1.3888888888888952E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15">
+    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>30</v>
       </c>
@@ -1882,254 +1926,386 @@
         <v>-0.7284722222222223</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15">
-      <c r="A10" s="18"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7">
+        <v>15</v>
+      </c>
+      <c r="C10" s="7">
+        <v>12</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.76041666666666663</v>
+      </c>
       <c r="G10" s="8">
         <f t="shared" si="1"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="H10" s="7">
         <v>0</v>
       </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
       <c r="J10" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15">
-      <c r="A11" s="18"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+        <v>1.736111111111116E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="7">
+        <v>12</v>
+      </c>
+      <c r="C11" s="7">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.76944444444444438</v>
+      </c>
       <c r="G11" s="8">
         <f t="shared" si="1"/>
+        <v>4.8611111111109828E-3</v>
+      </c>
+      <c r="H11" s="7">
         <v>0</v>
       </c>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
       <c r="J11" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15">
-      <c r="A12" s="18"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
+        <v>4.8611111111109828E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="7">
+        <v>6</v>
+      </c>
+      <c r="C12" s="7">
+        <v>8</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.7909722222222223</v>
+      </c>
       <c r="G12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
+        <v>9.0277777777778567E-3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
       <c r="J12" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15">
-      <c r="A13" s="18"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+        <v>1.9444444444444521E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="7">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7">
+        <v>24</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.81458333333333333</v>
+      </c>
       <c r="G13" s="8">
         <f t="shared" si="1"/>
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="H13" s="7">
         <v>0</v>
       </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="8"/>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
       <c r="J13" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15">
-      <c r="A14" s="19"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+        <v>8.3333333333333037E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="7">
+        <v>20</v>
+      </c>
+      <c r="C14" s="7">
+        <v>18</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.85902777777777783</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.87013888888888891</v>
+      </c>
       <c r="G14" s="8">
         <f t="shared" si="1"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="H14" s="7">
         <v>0</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
       <c r="J14" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="7">
+        <v>4</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.875</v>
+      </c>
       <c r="G15" s="8">
         <f t="shared" si="1"/>
+        <v>2.7777777777777679E-3</v>
+      </c>
+      <c r="H15" s="7">
         <v>0</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
       <c r="J15" s="30">
         <f t="shared" si="0"/>
+        <v>2.7777777777777679E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A16" s="48" t="s">
+      <c r="H16" s="7"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="24">
-        <f>SUM(B6:B15)</f>
-        <v>130</v>
-      </c>
-      <c r="C16" s="24">
-        <f>SUM(C6:C15)</f>
-        <v>81</v>
-      </c>
-      <c r="D16" s="25">
-        <f>SUM(D6:D15)</f>
-        <v>4.6527777777777779E-2</v>
-      </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25">
-        <f>SUM(G6:G15)</f>
-        <v>-0.68124999999999991</v>
-      </c>
-      <c r="H16" s="26">
-        <f>SUM(H6:H15)</f>
-        <v>1</v>
-      </c>
-      <c r="I16" s="27">
-        <f>SUM(I6:I15)</f>
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="J16" s="28">
-        <f>SUM(J6:J15)</f>
-        <v>-0.68055555555555547</v>
-      </c>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A17" s="49" t="s">
+      <c r="B18" s="24">
+        <f>SUM(B6:B17)</f>
+        <v>217</v>
+      </c>
+      <c r="C18" s="24">
+        <f>SUM(C6:C17)</f>
+        <v>159</v>
+      </c>
+      <c r="D18" s="25">
+        <f>SUM(D6:D17)</f>
+        <v>9.6527777777777782E-2</v>
+      </c>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25">
+        <f>SUM(G6:G17)</f>
+        <v>-0.62777777777777777</v>
+      </c>
+      <c r="H18" s="26">
+        <f>SUM(H6:H17)</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="27">
+        <f>SUM(I6:I17)</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="J18" s="28">
+        <f>SUM(J6:J17)</f>
+        <v>-0.6166666666666667</v>
+      </c>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="20">
-        <f>IF(EXACT($C$16, 0),"-",ABS($B$16-$C$16)/$C$16)</f>
-        <v>0.60493827160493829</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1"/>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A19" s="42" t="s">
+      <c r="B19" s="20">
+        <f>IF(EXACT($C$18, 0),"-",ABS($B$18-$C$18)/$C$18)</f>
+        <v>0.36477987421383645</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="43"/>
-    </row>
-    <row r="20" spans="1:10" ht="15">
-      <c r="A20" s="31" t="s">
+      <c r="B21" s="43"/>
+    </row>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="32">
-        <f>C16</f>
-        <v>81</v>
-      </c>
-      <c r="C20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="33" t="s">
+      <c r="B22" s="32">
+        <f>C18</f>
+        <v>159</v>
+      </c>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="34">
-        <f>IF(EXACT($B$20,0),"-",$B$20/((J16-INT(J16))*24))</f>
-        <v>10.565217391304344</v>
-      </c>
-      <c r="C21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A22" s="35" t="s">
+      <c r="B23" s="34">
+        <f>IF(EXACT($B$22,0),"-",$B$22/((J18-INT(J18))*24))</f>
+        <v>17.282608695652176</v>
+      </c>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="34">
-        <f>IF(EXACT($B$20,0),"-",H16/($B$20/10))</f>
-        <v>0.1234567901234568</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A23" s="35" t="s">
+      <c r="B24" s="34">
+        <f>IF(EXACT($B$22,0),"-",H18/($B$22/10))</f>
+        <v>0.12578616352201258</v>
+      </c>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="36">
-        <f>IF(EXACT($B$20,0),"-",H16/$B$20)</f>
-        <v>1.2345679012345678E-2</v>
-      </c>
-      <c r="C23" s="44" t="s">
+      <c r="B25" s="36">
+        <f>IF(EXACT($B$22,0),"-",H18/$B$22)</f>
+        <v>1.2578616352201259E-2</v>
+      </c>
+      <c r="C25" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="35" t="s">
+    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="37">
-        <f>I16</f>
-        <v>6.9444444444444447E-4</v>
-      </c>
-      <c r="C24" s="40">
-        <f>IF(EXACT(J16,0),5%,B24/J16)</f>
-        <v>-1.0204081632653062E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A25" s="38" t="s">
+      <c r="B26" s="37">
+        <f>I18</f>
+        <v>1.111111111111111E-2</v>
+      </c>
+      <c r="C26" s="40">
+        <f>IF(EXACT(J18,0),5%,B26/J18)</f>
+        <v>-1.8018018018018014E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="39">
-        <f>G16</f>
-        <v>-0.68124999999999991</v>
-      </c>
-      <c r="C25" s="41">
-        <f>IF(EXACT(J16,0),95%,B25/J16)</f>
-        <v>1.0010204081632652</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A26" s="38" t="s">
+      <c r="B27" s="39">
+        <f>G18</f>
+        <v>-0.62777777777777777</v>
+      </c>
+      <c r="C27" s="41">
+        <f>IF(EXACT(J18,0),95%,B27/J18)</f>
+        <v>1.0180180180180181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="39">
-        <f>C2+C3+J16</f>
-        <v>-0.6645833333333333</v>
-      </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="D27" s="6"/>
-    </row>
-    <row r="40" spans="3:4">
-      <c r="C40" s="4"/>
-    </row>
-    <row r="42" spans="3:4">
-      <c r="D42" s="4"/>
+      <c r="B28" s="39">
+        <f>C2+C3+J18</f>
+        <v>-0.60069444444444453</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D29" s="6"/>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Realizado el merge a pedido de los cambios de Hernán sobre los de Bruno: producto entre vectores, setColumna y setFila, restar, sumar, y producto en VectorFila y VectorColumna, mains en dichas clases, constructores en dichas clases. Agregadas también MatrizCuadrada y MatrizIdentidad. Actualizadas las métricas por un pequeño error (incompleto tiempo y LoC real en iteración "Metodos Norma 1, 2, inf en vector").
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas_sel.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas_sel.xlsx
@@ -1101,10 +1101,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-1.8018018018018014E-2</c:v>
+                  <c:v>9.3023255813953445E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0180180180180181</c:v>
+                  <c:v>0.90697674418604668</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1692,7 +1692,7 @@
   <dimension ref="A1:IU44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1703,7 +1703,7 @@
     <col min="4" max="4" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1901,7 +1901,9 @@
       <c r="B9" s="7">
         <v>20</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7">
+        <v>24</v>
+      </c>
       <c r="D9" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
@@ -1909,11 +1911,11 @@
         <v>0.7284722222222223</v>
       </c>
       <c r="F9" s="8">
-        <v>0</v>
+        <v>0.73611111111111116</v>
       </c>
       <c r="G9" s="8">
         <f t="shared" si="1"/>
-        <v>-0.7284722222222223</v>
+        <v>7.6388888888888618E-3</v>
       </c>
       <c r="H9" s="7">
         <v>0</v>
@@ -1923,7 +1925,7 @@
       </c>
       <c r="J9" s="30">
         <f t="shared" si="0"/>
-        <v>-0.7284722222222223</v>
+        <v>7.6388888888888618E-3</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2176,7 +2178,7 @@
       </c>
       <c r="C18" s="24">
         <f>SUM(C6:C17)</f>
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="D18" s="25">
         <f>SUM(D6:D17)</f>
@@ -2186,7 +2188,7 @@
       <c r="F18" s="24"/>
       <c r="G18" s="25">
         <f>SUM(G6:G17)</f>
-        <v>-0.62777777777777777</v>
+        <v>0.10833333333333339</v>
       </c>
       <c r="H18" s="26">
         <f>SUM(H6:H17)</f>
@@ -2198,7 +2200,7 @@
       </c>
       <c r="J18" s="28">
         <f>SUM(J6:J17)</f>
-        <v>-0.6166666666666667</v>
+        <v>0.11944444444444449</v>
       </c>
       <c r="K18" s="4"/>
     </row>
@@ -2208,7 +2210,7 @@
       </c>
       <c r="B19" s="20">
         <f>IF(EXACT($C$18, 0),"-",ABS($B$18-$C$18)/$C$18)</f>
-        <v>0.36477987421383645</v>
+        <v>0.18579234972677597</v>
       </c>
       <c r="D19" s="5"/>
       <c r="J19" s="3"/>
@@ -2226,7 +2228,7 @@
       </c>
       <c r="B22" s="32">
         <f>C18</f>
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="C22" s="9"/>
     </row>
@@ -2236,7 +2238,7 @@
       </c>
       <c r="B23" s="34">
         <f>IF(EXACT($B$22,0),"-",$B$22/((J18-INT(J18))*24))</f>
-        <v>17.282608695652176</v>
+        <v>63.837209302325554</v>
       </c>
       <c r="C23" s="9"/>
     </row>
@@ -2246,7 +2248,7 @@
       </c>
       <c r="B24" s="34">
         <f>IF(EXACT($B$22,0),"-",H18/($B$22/10))</f>
-        <v>0.12578616352201258</v>
+        <v>0.10928961748633879</v>
       </c>
       <c r="C24" s="9"/>
     </row>
@@ -2256,7 +2258,7 @@
       </c>
       <c r="B25" s="36">
         <f>IF(EXACT($B$22,0),"-",H18/$B$22)</f>
-        <v>1.2578616352201259E-2</v>
+        <v>1.092896174863388E-2</v>
       </c>
       <c r="C25" s="44" t="s">
         <v>19</v>
@@ -2272,7 +2274,7 @@
       </c>
       <c r="C26" s="40">
         <f>IF(EXACT(J18,0),5%,B26/J18)</f>
-        <v>-1.8018018018018014E-2</v>
+        <v>9.3023255813953445E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2281,11 +2283,11 @@
       </c>
       <c r="B27" s="39">
         <f>G18</f>
-        <v>-0.62777777777777777</v>
+        <v>0.10833333333333339</v>
       </c>
       <c r="C27" s="41">
         <f>IF(EXACT(J18,0),95%,B27/J18)</f>
-        <v>1.0180180180180181</v>
+        <v>0.90697674418604668</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2294,7 +2296,7 @@
       </c>
       <c r="B28" s="39">
         <f>C2+C3+J18</f>
-        <v>-0.60069444444444453</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="D28" s="6"/>
     </row>

</xml_diff>

<commit_message>
Refactoría general. Movidos métodos de normas de vectores a la clase padre (es el mismo código para ambas, no tiene sentido duplicar código). Creados métodos getters de filas y columnas para MatrizMath. Agregada validación de referencia en algunos lugares que faltaba. Cambiados los modificadores de acceso de los constructores que utilzan a MatrizMath como parámetro (escondiendo comportamiento). Actualizado el diagrama UML. Actualizadas las métricas.
</commit_message>
<xml_diff>
--- a/practica2/trunk/TDAs/doc/metricas_sel.xlsx
+++ b/practica2/trunk/TDAs/doc/metricas_sel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -124,7 +124,16 @@
     <t>Producto entre MatrizMath con VectorFila y VectorColumna</t>
   </si>
   <si>
-    <t>Metodos setFila y setColumna de la Clase MatrizMath</t>
+    <t>Métodos setFila y setColumna de la Clase MatrizMath</t>
+  </si>
+  <si>
+    <t>Excepciones básicas y validación</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Refactorización general</t>
   </si>
 </sst>
 </file>
@@ -675,7 +684,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -793,6 +802,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="4" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Énfasis5" xfId="1" builtinId="46"/>
@@ -1082,7 +1092,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Metricas!$A$26:$A$27</c:f>
+              <c:f>Metricas!$A$32:$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1096,15 +1106,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Metricas!$C$26:$C$27</c:f>
+              <c:f>Metricas!$C$32:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.3023255813953445E-2</c:v>
+                  <c:v>7.441860465116272E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.90697674418604668</c:v>
+                  <c:v>0.92558139534883732</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,13 +1156,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1689,10 +1699,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:IU44"/>
+  <dimension ref="A1:IU50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="34.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1734,7 +1744,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="11">
-        <v>20</v>
+        <v>1.7361111111111112E-2</v>
       </c>
       <c r="C2" s="11">
         <f>E2-D2</f>
@@ -1845,8 +1855,8 @@
       <c r="F7" s="8">
         <v>0.91805555555555562</v>
       </c>
-      <c r="G7" s="8">
-        <f>F7-E7</f>
+      <c r="G7" s="17">
+        <f t="shared" ref="G7:G23" si="0">F7-E7</f>
         <v>2.6388888888889017E-2</v>
       </c>
       <c r="H7" s="7">
@@ -1856,47 +1866,47 @@
         <v>0</v>
       </c>
       <c r="J7" s="30">
-        <f t="shared" ref="J7:J17" si="0">G7+I7</f>
+        <f t="shared" ref="J7:J23" si="1">G7+I7</f>
         <v>2.6388888888889017E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C8" s="7">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D8" s="8">
-        <v>1.7361111111111112E-2</v>
+        <v>1.3888888888888888E-2</v>
       </c>
       <c r="E8" s="8">
-        <v>0.71250000000000002</v>
+        <v>0.92708333333333337</v>
       </c>
       <c r="F8" s="8">
-        <v>0.72569444444444453</v>
-      </c>
-      <c r="G8" s="8">
-        <f t="shared" ref="G8:G17" si="1">F8-E8</f>
-        <v>1.3194444444444509E-2</v>
+        <v>0.93888888888888899</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>1.1805555555555625E-2</v>
       </c>
       <c r="H8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>6.9444444444444447E-4</v>
+        <v>0</v>
       </c>
       <c r="J8" s="30">
-        <f t="shared" si="0"/>
-        <v>1.3888888888888952E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.1805555555555625E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="7">
         <v>20</v>
@@ -1905,409 +1915,554 @@
         <v>24</v>
       </c>
       <c r="D9" s="8">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="J9" s="30">
+        <f t="shared" si="1"/>
+        <v>1.3888888888888952E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="7">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E10" s="8">
         <v>0.7284722222222223</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F10" s="8">
         <v>0.73611111111111116</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>7.6388888888888618E-3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30">
         <f t="shared" si="1"/>
         <v>7.6388888888888618E-3</v>
       </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="30">
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="7">
+        <v>15</v>
+      </c>
+      <c r="C11" s="7">
+        <v>12</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="G11" s="17">
         <f t="shared" si="0"/>
-        <v>7.6388888888888618E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="7">
-        <v>15</v>
-      </c>
-      <c r="C10" s="7">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8">
-        <v>1.3888888888888888E-2</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.74305555555555547</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="G10" s="8">
+        <v>1.736111111111116E-2</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
+      <c r="J11" s="30">
         <f t="shared" si="1"/>
         <v>1.736111111111116E-2</v>
       </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="30">
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7">
+        <v>12</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.76458333333333339</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.76944444444444438</v>
+      </c>
+      <c r="G12" s="17">
         <f t="shared" si="0"/>
-        <v>1.736111111111116E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7">
-        <v>12</v>
-      </c>
-      <c r="C11" s="7">
-        <v>12</v>
-      </c>
-      <c r="D11" s="8">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0.76458333333333339</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0.76944444444444438</v>
-      </c>
-      <c r="G11" s="8">
+        <v>4.8611111111109828E-3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="30">
         <f t="shared" si="1"/>
         <v>4.8611111111109828E-3</v>
       </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="30">
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6</v>
+      </c>
+      <c r="C13" s="7">
+        <v>8</v>
+      </c>
+      <c r="D13" s="8">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.78194444444444444</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.7909722222222223</v>
+      </c>
+      <c r="G13" s="17">
         <f t="shared" si="0"/>
-        <v>4.8611111111109828E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="7">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7">
-        <v>8</v>
-      </c>
-      <c r="D12" s="8">
-        <v>6.9444444444444441E-3</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0.78194444444444444</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0.7909722222222223</v>
-      </c>
-      <c r="G12" s="8">
+        <v>9.0277777777778567E-3</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="J13" s="30">
         <f t="shared" si="1"/>
-        <v>9.0277777777778567E-3</v>
-      </c>
-      <c r="H12" s="7">
-        <v>1</v>
-      </c>
-      <c r="I12" s="8">
+        <v>1.9444444444444521E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="7">
+        <v>30</v>
+      </c>
+      <c r="C14" s="7">
+        <v>24</v>
+      </c>
+      <c r="D14" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="J12" s="30">
+      <c r="E14" s="8">
+        <v>0.80625000000000002</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.81458333333333333</v>
+      </c>
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
-        <v>1.9444444444444521E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="7">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7">
-        <v>24</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.80625000000000002</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0.81458333333333333</v>
-      </c>
-      <c r="G13" s="8">
+        <v>8.3333333333333037E-3</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="30">
         <f t="shared" si="1"/>
         <v>8.3333333333333037E-3</v>
       </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="30">
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="7">
+        <v>20</v>
+      </c>
+      <c r="C15" s="7">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.85902777777777783</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.87013888888888891</v>
+      </c>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
-        <v>8.3333333333333037E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="7">
-        <v>20</v>
-      </c>
-      <c r="C14" s="7">
-        <v>18</v>
-      </c>
-      <c r="D14" s="8">
-        <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0.85902777777777783</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.87013888888888891</v>
-      </c>
-      <c r="G14" s="8">
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="30">
         <f t="shared" si="1"/>
         <v>1.1111111111111072E-2</v>
       </c>
-      <c r="H14" s="7">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <v>0</v>
-      </c>
-      <c r="J14" s="30">
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.87222222222222223</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.875</v>
+      </c>
+      <c r="G16" s="17">
         <f t="shared" si="0"/>
-        <v>1.1111111111111072E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="7">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7">
-        <v>4</v>
-      </c>
-      <c r="D15" s="8">
-        <v>1.3888888888888889E-3</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.87222222222222223</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0.875</v>
-      </c>
-      <c r="G15" s="8">
+        <v>2.7777777777777679E-3</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="30">
         <f t="shared" si="1"/>
         <v>2.7777777777777679E-3</v>
       </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="8">
-        <v>0</v>
-      </c>
-      <c r="J15" s="30">
+    </row>
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E17" s="8">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="F17" s="8">
+        <v>8.7500000000000008E-2</v>
+      </c>
+      <c r="G17" s="17">
         <f t="shared" si="0"/>
-        <v>2.7777777777777679E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8">
+        <v>1.8055555555555575E-2</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="30">
+        <v>1.8055555555555575E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="53"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="8">
+      <c r="H18" s="22"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="30">
+    </row>
+    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="53"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="H19" s="22"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="53"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="53"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="53"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="24">
-        <f>SUM(B6:B17)</f>
-        <v>217</v>
-      </c>
-      <c r="C18" s="24">
-        <f>SUM(C6:C17)</f>
-        <v>183</v>
-      </c>
-      <c r="D18" s="25">
-        <f>SUM(D6:D17)</f>
-        <v>9.6527777777777782E-2</v>
-      </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25">
-        <f>SUM(G6:G17)</f>
-        <v>0.10833333333333339</v>
-      </c>
-      <c r="H18" s="26">
-        <f>SUM(H6:H17)</f>
+      <c r="B24" s="24">
+        <f>SUM(B6:B23)</f>
+        <v>267</v>
+      </c>
+      <c r="C24" s="24">
+        <f>SUM(C6:C23)</f>
+        <v>239</v>
+      </c>
+      <c r="D24" s="25">
+        <f>SUM(D6:D23)</f>
+        <v>0.12083333333333333</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="25">
+        <f>SUM(G6:G23)</f>
+        <v>0.13819444444444459</v>
+      </c>
+      <c r="H24" s="26">
+        <f>SUM(H6:H23)</f>
         <v>2</v>
       </c>
-      <c r="I18" s="27">
-        <f>SUM(I6:I17)</f>
+      <c r="I24" s="27">
+        <f>SUM(I6:I23)</f>
         <v>1.111111111111111E-2</v>
       </c>
-      <c r="J18" s="28">
-        <f>SUM(J6:J17)</f>
-        <v>0.11944444444444449</v>
-      </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49" t="s">
+      <c r="J24" s="28">
+        <f>SUM(J6:J23)</f>
+        <v>0.14930555555555569</v>
+      </c>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="20">
-        <f>IF(EXACT($C$18, 0),"-",ABS($B$18-$C$18)/$C$18)</f>
-        <v>0.18579234972677597</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="B25" s="20">
+        <f>IF(EXACT($C$24, 0),"-",ABS($B$24-$C$24)/$C$24)</f>
+        <v>0.11715481171548117</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="43"/>
-    </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="B27" s="43"/>
+    </row>
+    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="32">
-        <f>C18</f>
-        <v>183</v>
-      </c>
-      <c r="C22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="33" t="s">
+      <c r="B28" s="32">
+        <f>C24</f>
+        <v>239</v>
+      </c>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="34">
-        <f>IF(EXACT($B$22,0),"-",$B$22/((J18-INT(J18))*24))</f>
-        <v>63.837209302325554</v>
-      </c>
-      <c r="C23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="B29" s="34">
+        <f>IF(EXACT($B$28,0),"-",$B$28/((J24-INT(J24))*24))</f>
+        <v>66.697674418604592</v>
+      </c>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="34">
-        <f>IF(EXACT($B$22,0),"-",H18/($B$22/10))</f>
-        <v>0.10928961748633879</v>
-      </c>
-      <c r="C24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="35" t="s">
+      <c r="B30" s="34">
+        <f>IF(EXACT($B$28,0),"-",H24/($B$28/10))</f>
+        <v>8.3682008368200847E-2</v>
+      </c>
+      <c r="C30" s="9"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="36">
-        <f>IF(EXACT($B$22,0),"-",H18/$B$22)</f>
-        <v>1.092896174863388E-2</v>
-      </c>
-      <c r="C25" s="44" t="s">
+      <c r="B31" s="36">
+        <f>IF(EXACT($B$28,0),"-",H24/$B$28)</f>
+        <v>8.368200836820083E-3</v>
+      </c>
+      <c r="C31" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="37">
-        <f>I18</f>
+      <c r="B32" s="37">
+        <f>I24</f>
         <v>1.111111111111111E-2</v>
       </c>
-      <c r="C26" s="40">
-        <f>IF(EXACT(J18,0),5%,B26/J18)</f>
-        <v>9.3023255813953445E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="38" t="s">
+      <c r="C32" s="40">
+        <f>IF(EXACT(J24,0),5%,B32/J24)</f>
+        <v>7.441860465116272E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="39">
-        <f>G18</f>
-        <v>0.10833333333333339</v>
-      </c>
-      <c r="C27" s="41">
-        <f>IF(EXACT(J18,0),95%,B27/J18)</f>
-        <v>0.90697674418604668</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="B33" s="39">
+        <f>G24</f>
+        <v>0.13819444444444459</v>
+      </c>
+      <c r="C33" s="41">
+        <f>IF(EXACT(J24,0),95%,B33/J24)</f>
+        <v>0.92558139534883732</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="39">
-        <f>C2+C3+J18</f>
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D29" s="6"/>
-    </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C42" s="4"/>
-    </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D44" s="4"/>
+      <c r="B34" s="39">
+        <f>C2+C3+J24</f>
+        <v>0.16527777777777786</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="1">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="4"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>